<commit_message>
Delta Program : Debugging and Finalized Code
</commit_message>
<xml_diff>
--- a/Master2.xlsx
+++ b/Master2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/j_vorathammaporn_accenture_com/Documents/Desktop/Internship_Workspace/SandBox_Test/test_delta/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/j_a_vorathammaporn_accenture_com/Documents/Desktop/PTT-WorkSpace/Accenture-Data-Migration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{5CD0A33D-4AA8-4F85-ACF6-E1636C8AEB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99CA6268-4423-433B-853D-6A8015E06E98}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{5CD0A33D-4AA8-4F85-ACF6-E1636C8AEB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0119120C-E7E2-404C-929E-69AC75AE4EEE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5553D876-8CE6-4031-8D37-2253051AB329}"/>
   </bookViews>
@@ -94,9 +94,6 @@
     <t>Sheet1</t>
   </si>
   <si>
-    <t>C:\Users\j.vorathammaporn\OneDrive - Accenture\Desktop\Internship_Workspace\SandBox_Test\test_delta\</t>
-  </si>
-  <si>
     <t>firstRowOfData</t>
   </si>
   <si>
@@ -115,7 +112,10 @@
     <t>headerRow</t>
   </si>
   <si>
-    <t>Before_Delta_0023.xlsx</t>
+    <t>C:\Users\j.a.vorathammaporn\OneDrive - Accenture\Desktop\PTT-WorkSpace\Accenture-Data-Migration\</t>
+  </si>
+  <si>
+    <t>Master2.xlsx</t>
   </si>
 </sst>
 </file>
@@ -815,7 +815,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="58.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -836,7 +836,7 @@
     </row>
     <row r="2" spans="1:4" ht="39" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>18</v>
@@ -969,7 +969,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -987,7 +987,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="4">
         <v>9</v>
@@ -995,7 +995,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4">
         <v>4</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4">
         <v>5</v>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="4">
         <v>6</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="4">
         <v>8</v>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4">
         <v>5</v>
@@ -1144,12 +1144,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1291,24 +1288,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{372C0842-4D4A-446D-8B45-AE815A5DAA02}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D3FBD79-3017-4DAB-9132-325B92A4D8A3}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A630574-B6C5-4FE9-AFE1-1071C5FE6BAC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1319,6 +1307,32 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D3FBD79-3017-4DAB-9132-325B92A4D8A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2f423150-2cdd-48d9-9270-a69c1f7e699a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{372C0842-4D4A-446D-8B45-AE815A5DAA02}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>